<commit_message>
Agregando riesgo identificado en proceso
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Planeacion/Plan_riesgos.xlsx
+++ b/qualtcom/Procesos/Planeacion/Plan_riesgos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Procesos\Planeacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\qualtcom\Procesos\Planeacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>Abierto</t>
+  </si>
+  <si>
+    <t>Acceso denegado al dispositivo de respaldo</t>
+  </si>
+  <si>
+    <t>Generar adquisicion de un dispositivo secundario que lea discos duros del actual</t>
+  </si>
+  <si>
+    <t>Solicitar al usuario cargar en usb la informacion mas reciente que ha generado</t>
   </si>
 </sst>
 </file>
@@ -643,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,23 +988,39 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.15</v>
+      </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="5"/>
+        <v>0.6</v>
+      </c>
+      <c r="G14" s="5">
+        <v>4</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="5">

</xml_diff>

<commit_message>
Actualizacion del plan de riesgo(status de riesgos)
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Planeacion/Plan_riesgos.xlsx
+++ b/qualtcom/Procesos/Planeacion/Plan_riesgos.xlsx
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +815,7 @@
         <v>12</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="45" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
         <v>12</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="60" x14ac:dyDescent="0.25">
@@ -917,7 +917,7 @@
         <v>30</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="45" x14ac:dyDescent="0.25">
@@ -985,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizacion del plan de riesgos
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Planeacion/Plan_riesgos.xlsx
+++ b/qualtcom/Procesos/Planeacion/Plan_riesgos.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>PLAN DE RIESGOS</t>
   </si>
@@ -211,7 +211,10 @@
     <t>Solicitar al usuario cargar en usb la informacion mas reciente que ha generado</t>
   </si>
   <si>
-    <t>Ocurrido en Junio por problema de clima</t>
+    <t>Se presenta una pequena desviacion en julio por un mes mas largo</t>
+  </si>
+  <si>
+    <t>Ocurrido en Junio por problema de clima, presentado en martes 28 Julio.</t>
   </si>
 </sst>
 </file>
@@ -316,12 +319,6 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,6 +365,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -743,26 +746,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="3"/>
-    <col min="2" max="2" width="3" style="4"/>
-    <col min="3" max="3" width="35.5703125" style="5"/>
-    <col min="4" max="7" width="14.28515625" style="4"/>
-    <col min="8" max="9" width="35.5703125" style="3"/>
-    <col min="10" max="11" width="14.28515625" style="3"/>
-    <col min="12" max="12" width="18.42578125" style="3"/>
-    <col min="13" max="1025" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="2.85546875" style="1"/>
+    <col min="2" max="2" width="3" style="2"/>
+    <col min="3" max="3" width="35.5703125" style="3"/>
+    <col min="4" max="7" width="14.28515625" style="2"/>
+    <col min="8" max="9" width="35.5703125" style="1"/>
+    <col min="10" max="11" width="14.28515625" style="1"/>
+    <col min="12" max="12" width="18.42578125" style="1"/>
+    <col min="13" max="1025" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
@@ -784,18 +787,18 @@
       <c r="K2"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="B3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4"/>
@@ -810,833 +813,835 @@
       <c r="K4"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L5" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>3</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <v>0.4</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <f t="shared" ref="F6:F40" si="0">D6*E6</f>
         <v>1.2000000000000002</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>2</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="17"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <f t="shared" ref="B7:B40" si="1">B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>5</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>0.3</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>1</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="17"/>
+      <c r="L7" s="15"/>
     </row>
     <row r="8" spans="2:12" ht="59.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>5</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>0.2</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <v>2</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>0.65</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>1.3</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <v>2</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <v>2</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="8">
         <v>0.45</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <v>3</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="16" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <v>4</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="8">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="6">
         <v>1</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
+    <row r="12" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>3</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="8">
         <v>0.6</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>1</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="17"/>
+      <c r="L12" s="17" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>5</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="8">
         <v>0.15</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="6">
         <v>3</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="18" t="s">
+      <c r="L13" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="8">
+    <row r="14" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="8">
         <v>0.15</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="6">
         <v>3</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="18" t="s">
-        <v>48</v>
+      <c r="L14" s="16" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="12"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="12"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="6"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="12"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="14"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="12"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="12"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="14"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="12"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="8">
+      <c r="B22" s="6">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="14"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="12"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="8">
+      <c r="B23" s="6">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="14"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="12"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="8">
+      <c r="B24" s="6">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="14"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="12"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="8">
+      <c r="B25" s="6">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="14"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="8">
+      <c r="B26" s="6">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="14"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="12"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="8">
+      <c r="B27" s="6">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="14"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="8">
+      <c r="B28" s="6">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="14"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="8">
+      <c r="B29" s="6">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="14"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="12"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="12"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="8">
+      <c r="B31" s="6">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="14"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="12"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="8">
+      <c r="B32" s="6">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="12"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="8">
+      <c r="B33" s="6">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="14"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="12"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="8">
+      <c r="B34" s="6">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="14"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="6"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="12"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="8">
+      <c r="B35" s="6">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="14"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="12"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="8">
+      <c r="B36" s="6">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="8"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="14"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="12"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="8">
+      <c r="B37" s="6">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="8"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="14"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="12"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="8">
+      <c r="B38" s="6">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="14"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="12"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="8">
+      <c r="B39" s="6">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G39" s="8"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="14"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="12"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="8">
+      <c r="B40" s="6">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="13"/>
-      <c r="K40" s="14"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>